<commit_message>
Added tableau map and made changes to median income data
</commit_message>
<xml_diff>
--- a/Median-household-income/median-master.xlsx
+++ b/Median-household-income/median-master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataVis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataVis\DataVis-Coronavirus\Median-household-income\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFAF35C-FF49-4BC5-BF70-B37F327E0BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935982EB-1C6F-481D-8C11-FF62057A5AC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C759F746-DBDB-4E11-95CA-439512B4D96F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>Battery Park/Tribeca</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Boro Cd</t>
   </si>
 </sst>
 </file>
@@ -305,12 +308,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -628,14 +636,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D65A5A5-9841-48FC-84C7-E8B0320B964C}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" style="5" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" customWidth="1"/>
   </cols>
@@ -644,8 +652,8 @@
       <c r="A1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+      <c r="B1" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>70</v>
@@ -658,6 +666,7 @@
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
@@ -669,6 +678,9 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="5">
+        <v>101</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -680,6 +692,9 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="5">
+        <v>102</v>
+      </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
@@ -691,6 +706,9 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="5">
+        <v>103</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -702,6 +720,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="5">
+        <v>104</v>
+      </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -713,6 +734,9 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7" s="5">
+        <v>105</v>
+      </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -724,6 +748,9 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8" s="5">
+        <v>106</v>
+      </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
@@ -735,6 +762,9 @@
       <c r="A9" t="s">
         <v>67</v>
       </c>
+      <c r="B9" s="5">
+        <v>107</v>
+      </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -746,6 +776,9 @@
       <c r="A10" t="s">
         <v>66</v>
       </c>
+      <c r="B10" s="5">
+        <v>108</v>
+      </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -757,6 +790,9 @@
       <c r="A11" t="s">
         <v>65</v>
       </c>
+      <c r="B11" s="5">
+        <v>109</v>
+      </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
@@ -768,6 +804,9 @@
       <c r="A12" t="s">
         <v>64</v>
       </c>
+      <c r="B12" s="5">
+        <v>110</v>
+      </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -779,6 +818,9 @@
       <c r="A13" t="s">
         <v>63</v>
       </c>
+      <c r="B13" s="5">
+        <v>111</v>
+      </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -790,6 +832,9 @@
       <c r="A14" t="s">
         <v>62</v>
       </c>
+      <c r="B14" s="5">
+        <v>112</v>
+      </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
@@ -801,6 +846,7 @@
       <c r="A15" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
@@ -812,6 +858,9 @@
       <c r="A16" t="s">
         <v>60</v>
       </c>
+      <c r="B16" s="5">
+        <v>201</v>
+      </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
@@ -823,6 +872,9 @@
       <c r="A17" t="s">
         <v>59</v>
       </c>
+      <c r="B17" s="5">
+        <v>202</v>
+      </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
@@ -834,6 +886,9 @@
       <c r="A18" t="s">
         <v>58</v>
       </c>
+      <c r="B18" s="5">
+        <v>203</v>
+      </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
@@ -845,6 +900,9 @@
       <c r="A19" t="s">
         <v>57</v>
       </c>
+      <c r="B19" s="5">
+        <v>204</v>
+      </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
@@ -856,6 +914,9 @@
       <c r="A20" t="s">
         <v>56</v>
       </c>
+      <c r="B20" s="5">
+        <v>205</v>
+      </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
@@ -867,6 +928,9 @@
       <c r="A21" t="s">
         <v>55</v>
       </c>
+      <c r="B21" s="5">
+        <v>206</v>
+      </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
@@ -878,6 +942,9 @@
       <c r="A22" t="s">
         <v>54</v>
       </c>
+      <c r="B22" s="5">
+        <v>207</v>
+      </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
@@ -889,6 +956,9 @@
       <c r="A23" t="s">
         <v>53</v>
       </c>
+      <c r="B23" s="5">
+        <v>208</v>
+      </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
@@ -900,6 +970,9 @@
       <c r="A24" t="s">
         <v>52</v>
       </c>
+      <c r="B24" s="5">
+        <v>209</v>
+      </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
@@ -911,6 +984,9 @@
       <c r="A25" t="s">
         <v>51</v>
       </c>
+      <c r="B25" s="5">
+        <v>210</v>
+      </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
@@ -922,6 +998,9 @@
       <c r="A26" t="s">
         <v>50</v>
       </c>
+      <c r="B26" s="5">
+        <v>211</v>
+      </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
@@ -933,6 +1012,9 @@
       <c r="A27" t="s">
         <v>49</v>
       </c>
+      <c r="B27" s="5">
+        <v>212</v>
+      </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
@@ -944,6 +1026,7 @@
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
@@ -955,6 +1038,9 @@
       <c r="A29" t="s">
         <v>47</v>
       </c>
+      <c r="B29" s="5">
+        <v>301</v>
+      </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
@@ -966,6 +1052,9 @@
       <c r="A30" t="s">
         <v>46</v>
       </c>
+      <c r="B30" s="5">
+        <v>302</v>
+      </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
@@ -977,6 +1066,9 @@
       <c r="A31" t="s">
         <v>45</v>
       </c>
+      <c r="B31" s="5">
+        <v>303</v>
+      </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
@@ -988,6 +1080,9 @@
       <c r="A32" t="s">
         <v>44</v>
       </c>
+      <c r="B32" s="5">
+        <v>304</v>
+      </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
@@ -999,6 +1094,9 @@
       <c r="A33" t="s">
         <v>43</v>
       </c>
+      <c r="B33" s="5">
+        <v>305</v>
+      </c>
       <c r="C33" t="s">
         <v>10</v>
       </c>
@@ -1010,6 +1108,9 @@
       <c r="A34" t="s">
         <v>42</v>
       </c>
+      <c r="B34" s="5">
+        <v>306</v>
+      </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
@@ -1021,6 +1122,9 @@
       <c r="A35" t="s">
         <v>41</v>
       </c>
+      <c r="B35" s="5">
+        <v>307</v>
+      </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
@@ -1032,6 +1136,9 @@
       <c r="A36" t="s">
         <v>40</v>
       </c>
+      <c r="B36" s="5">
+        <v>308</v>
+      </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
@@ -1043,6 +1150,9 @@
       <c r="A37" t="s">
         <v>39</v>
       </c>
+      <c r="B37" s="5">
+        <v>309</v>
+      </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
@@ -1054,6 +1164,9 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
+      <c r="B38" s="5">
+        <v>310</v>
+      </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
@@ -1065,6 +1178,9 @@
       <c r="A39" t="s">
         <v>37</v>
       </c>
+      <c r="B39" s="5">
+        <v>311</v>
+      </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
@@ -1076,6 +1192,9 @@
       <c r="A40" t="s">
         <v>36</v>
       </c>
+      <c r="B40" s="5">
+        <v>312</v>
+      </c>
       <c r="C40" t="s">
         <v>10</v>
       </c>
@@ -1087,6 +1206,9 @@
       <c r="A41" t="s">
         <v>35</v>
       </c>
+      <c r="B41" s="5">
+        <v>313</v>
+      </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
@@ -1098,6 +1220,9 @@
       <c r="A42" t="s">
         <v>34</v>
       </c>
+      <c r="B42" s="5">
+        <v>314</v>
+      </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
@@ -1109,6 +1234,9 @@
       <c r="A43" t="s">
         <v>33</v>
       </c>
+      <c r="B43" s="5">
+        <v>315</v>
+      </c>
       <c r="C43" t="s">
         <v>10</v>
       </c>
@@ -1120,6 +1248,9 @@
       <c r="A44" t="s">
         <v>32</v>
       </c>
+      <c r="B44" s="5">
+        <v>316</v>
+      </c>
       <c r="C44" t="s">
         <v>10</v>
       </c>
@@ -1131,6 +1262,9 @@
       <c r="A45" t="s">
         <v>31</v>
       </c>
+      <c r="B45" s="5">
+        <v>317</v>
+      </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
@@ -1142,6 +1276,9 @@
       <c r="A46" t="s">
         <v>30</v>
       </c>
+      <c r="B46" s="5">
+        <v>318</v>
+      </c>
       <c r="C46" t="s">
         <v>10</v>
       </c>
@@ -1153,6 +1290,7 @@
       <c r="A47" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B47" s="4"/>
       <c r="C47" s="2" t="s">
         <v>10</v>
       </c>
@@ -1164,6 +1302,9 @@
       <c r="A48" t="s">
         <v>28</v>
       </c>
+      <c r="B48" s="5">
+        <v>401</v>
+      </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
@@ -1175,6 +1316,9 @@
       <c r="A49" t="s">
         <v>27</v>
       </c>
+      <c r="B49" s="5">
+        <v>402</v>
+      </c>
       <c r="C49" t="s">
         <v>10</v>
       </c>
@@ -1186,6 +1330,9 @@
       <c r="A50" t="s">
         <v>26</v>
       </c>
+      <c r="B50" s="5">
+        <v>403</v>
+      </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
@@ -1197,6 +1344,9 @@
       <c r="A51" t="s">
         <v>25</v>
       </c>
+      <c r="B51" s="5">
+        <v>404</v>
+      </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
@@ -1208,6 +1358,9 @@
       <c r="A52" t="s">
         <v>24</v>
       </c>
+      <c r="B52" s="5">
+        <v>405</v>
+      </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
@@ -1219,6 +1372,9 @@
       <c r="A53" t="s">
         <v>23</v>
       </c>
+      <c r="B53" s="5">
+        <v>406</v>
+      </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
@@ -1230,6 +1386,9 @@
       <c r="A54" t="s">
         <v>22</v>
       </c>
+      <c r="B54" s="5">
+        <v>407</v>
+      </c>
       <c r="C54" t="s">
         <v>10</v>
       </c>
@@ -1241,6 +1400,9 @@
       <c r="A55" t="s">
         <v>21</v>
       </c>
+      <c r="B55" s="5">
+        <v>408</v>
+      </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
@@ -1252,6 +1414,9 @@
       <c r="A56" t="s">
         <v>20</v>
       </c>
+      <c r="B56" s="5">
+        <v>409</v>
+      </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
@@ -1263,6 +1428,9 @@
       <c r="A57" t="s">
         <v>19</v>
       </c>
+      <c r="B57" s="5">
+        <v>410</v>
+      </c>
       <c r="C57" t="s">
         <v>10</v>
       </c>
@@ -1274,6 +1442,9 @@
       <c r="A58" t="s">
         <v>18</v>
       </c>
+      <c r="B58" s="5">
+        <v>411</v>
+      </c>
       <c r="C58" t="s">
         <v>10</v>
       </c>
@@ -1285,6 +1456,9 @@
       <c r="A59" t="s">
         <v>17</v>
       </c>
+      <c r="B59" s="5">
+        <v>412</v>
+      </c>
       <c r="C59" t="s">
         <v>10</v>
       </c>
@@ -1296,6 +1470,9 @@
       <c r="A60" t="s">
         <v>16</v>
       </c>
+      <c r="B60" s="5">
+        <v>413</v>
+      </c>
       <c r="C60" t="s">
         <v>10</v>
       </c>
@@ -1307,6 +1484,9 @@
       <c r="A61" t="s">
         <v>15</v>
       </c>
+      <c r="B61" s="5">
+        <v>414</v>
+      </c>
       <c r="C61" t="s">
         <v>10</v>
       </c>
@@ -1318,6 +1498,7 @@
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B62" s="4"/>
       <c r="C62" s="2" t="s">
         <v>10</v>
       </c>
@@ -1329,6 +1510,9 @@
       <c r="A63" t="s">
         <v>13</v>
       </c>
+      <c r="B63" s="5">
+        <v>501</v>
+      </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
@@ -1340,6 +1524,9 @@
       <c r="A64" t="s">
         <v>12</v>
       </c>
+      <c r="B64" s="5">
+        <v>502</v>
+      </c>
       <c r="C64" t="s">
         <v>10</v>
       </c>
@@ -1351,6 +1538,9 @@
       <c r="A65" t="s">
         <v>11</v>
       </c>
+      <c r="B65" s="5">
+        <v>503</v>
+      </c>
       <c r="C65" t="s">
         <v>10</v>
       </c>
@@ -1360,6 +1550,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1367,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDBEDE0-B6D8-46E5-88DA-5ACCDDABFD79}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>